<commit_message>
bug fixes in auctioneer, prices and dates
</commit_message>
<xml_diff>
--- a/output/leilaoimoveis.xlsx
+++ b/output/leilaoimoveis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Área Total</t>
+          <t>Área Total [m²]</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Área Útil</t>
+          <t>Área Útil [m²]</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -501,257 +501,141 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>Matrícula</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Inscrição Imobiliária</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>Localização</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>209.535,20</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>150,00 m²</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>130,00 m²</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>209535.2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>150</v>
+      </c>
+      <c r="C2" t="n">
+        <v>130</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>331.170,00</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>331170</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>18/11/2021</t>
+        </is>
+      </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr">
         <is>
+          <t>62166</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>5533031</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
           <t>RUA ELISEU ORIA (ANTIGA RUA JOSE MARIO MAMEDE),N. 179, JOSE DE ALENCAR - CEP: 60000-000, FORTALEZA - CEARA</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-jose-de-alencar-3-quartos-1-vaga-na-garagem-area-de-servico-2-wc-sala-co-imovel-caixa-economica-federal-cef-853865-1444408651124-venda-direta-caixa</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>555.000,00</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>72,91 m²</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>555.000,00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
+      <c r="A3" t="n">
+        <v>720000</v>
+      </c>
+      <c r="B3" t="n">
+        <v>250</v>
+      </c>
+      <c r="C3" t="n">
+        <v>121</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>720000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>432000</v>
+      </c>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>29/02/2024</t>
+        </is>
+      </c>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>29/04/2024</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
+          <t>03/06/2024</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>12/06/2024</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>RUA OSVALDO CRUZ N 3311 504,N. 3311 APTO. 504 0, TAUAPE - CEP: 60120-325, FORTALEZA - CEARA</t>
+          <t>73457</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-edificio-preludio-4-quartos-3-vagas-na-garagem-3-wc-wc-emp-sala-cozinha-imovel-caixa-economica-federal-cef-1613969-1555533013970-venda-direta-caixa</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>260.000,00</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>85,81 m²</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>260.000,00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>23/04/2024</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>RUA PROFESSOR MOREIRA DE SOUZA NUMERO 397 CASA 20,N. 397 CASA 20, PASSARE - CEP: 60862-040, FORTALEZA - CEARA</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-loteamento-parque-estrela-5-quartos-2-vagas-na-garagem-5-wc-wc-emp-sala-imovel-caixa-economica-federal-cef-1613967-1444408603073-venda-direta-caixa</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>210.000,00</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>61,24 m²</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>210.000,00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>30/04/2024</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>RUA ANTONINA DO NORTE N 194 446 04,N. 194 APTO. 446 BL04, SAO GERARDO - CEP: 60325-610, FORTALEZA - CEARA</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-monte-castelo-5-quartos-1-vaga-na-garagem-area-de-servico-4-wc-sala-imovel-caixa-economica-federal-cef-1613966-8444403365814-venda-direta-caixa</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>275.560,00</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>63,09 m²</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>275.560,00</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>29/04/2024</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>RUA AMANCIO VALENTE N 1555 202 03,N. 1555 APTO. 202 BLOBO 03, CAMBEBA - CEP: 60822-155, FORTALEZA - CEARA</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-favoritto-residence-clube-3-quartos-1-vaga-na-garagem-3-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1613965-1555538321207-venda-direta-caixa</t>
+          <t>5045363</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>RUA MARIA ALMEIDA ANTIGA RUA 03,N. 427 TERRENO 23A, COACU - CEP: 60871-742, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-coacu-6-quartos-7-wc-wc-emp-4-salas-cozinha-imovel-caixa-economica-federal-cef-1620167-1188800008524-venda-direta-caixa</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed number of pages
</commit_message>
<xml_diff>
--- a/output/leilaoimoveis.xlsx
+++ b/output/leilaoimoveis.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -639,6 +639,2292 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>555000</v>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>72.91</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>555000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>446300.19</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>26/02/2024</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>29/04/2024</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>08/05/2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>41931</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>8241899</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>RUA OSVALDO CRUZ N 3311 504,N. 3311 APTO. 504 0, TAUAPE - CEP: 60120-325, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-edificio-preludio-4-quartos-3-vagas-na-garagem-3-wc-wc-emp-sala-cozinha-imovel-caixa-economica-federal-cef-1613969-1555533013970-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>260000</v>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>85.81</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>260000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>255290.77</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>26/02/2024</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>23/04/2024</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>02/05/2024</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>53061</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>8012393</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>RUA PROFESSOR MOREIRA DE SOUZA NUMERO 397 CASA 20,N. 397 CASA 20, PASSARE - CEP: 60862-040, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-loteamento-parque-estrela-5-quartos-2-vagas-na-garagem-5-wc-wc-emp-sala-imovel-caixa-economica-federal-cef-1613967-1444408603073-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>210000</v>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="n">
+        <v>61.24</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>210000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>271605.48</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>26/02/2024</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>30/04/2024</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>09/05/2024</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>45073</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>RUA ANTONINA DO NORTE N 194 446 04,N. 194 APTO. 446 BL04, SAO GERARDO - CEP: 60325-610, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-monte-castelo-5-quartos-1-vaga-na-garagem-area-de-servico-4-wc-sala-imovel-caixa-economica-federal-cef-1613966-8444403365814-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>275560</v>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="n">
+        <v>63.09</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="n">
+        <v>275560</v>
+      </c>
+      <c r="G7" t="n">
+        <v>315079.59</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>26/02/2024</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>29/04/2024</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>08/05/2024</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>19710</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>8272980</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>RUA AMANCIO VALENTE N 1555 202 03,N. 1555 APTO. 202 BLOBO 03, CAMBEBA - CEP: 60822-155, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-favoritto-residence-clube-3-quartos-1-vaga-na-garagem-3-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1613965-1555538321207-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>300050.5</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>61.8</v>
+      </c>
+      <c r="D8" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>300050.5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>230256.13</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>26/02/2024</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>29/04/2024</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>08/05/2024</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>54067</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>8207410</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>RUA DAS CARNAUBAS N 441 501 ED ARACA,N. 441 APTO. 501 BLOCO B2, PASSARE - CEP: 60743-780, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-reserva-passare-condominio-park-iii-4-quartos-2-vagas-na-garagem-3-wc-sal-imovel-caixa-economica-federal-cef-1613963-1555534680873-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>187090</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>55.06</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>187090</v>
+      </c>
+      <c r="G9" t="n">
+        <v>92400</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>15/04/2024</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>24/04/2024</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>27853</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>RUA MAPIRUNGA,N. 85 APTO. 301 BL B, MARAPONGA - CEP: 60714-190, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-resid-recanto-da-maraponga-4-quartos-area-de-servico-3-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1605334-8057890000066-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>290000</v>
+      </c>
+      <c r="B10" t="n">
+        <v>198</v>
+      </c>
+      <c r="C10" t="n">
+        <v>130</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>290000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>174406.58</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>15/04/2024</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>24/04/2024</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>75213</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>RUA MAXIMINO,N. 215 T10 QD 05, MESSEJANA - CEP: 60830-555, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-loteam-santo-antonio-de-muriti-5-quartos-2-vagas-na-garagem-5-wc-sala-co-imovel-caixa-economica-federal-cef-1605332-1555507294909-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>207690</v>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="n">
+        <v>60</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
+        <v>207690</v>
+      </c>
+      <c r="G11" t="n">
+        <v>133459.96</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>15/04/2024</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>24/04/2024</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>83245</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>7383223</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>RUA GARDENIA,N. 603 APTO. 104 TP B 1PAV, PAUPINA - CEP: 60872-675, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-hesed-residence-3-quartos-1-vaga-na-garagem-3-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1605328-8444403236593-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>663766</v>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="n">
+        <v>155.02</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>663766</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1024177.03</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>14/02/2024</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>10/04/2024</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>85246</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>7140649</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>RUA BILL CARTAXO N 461,N. 461 CS 11 TIPO A, SAPIRANGACOITE - CEP: 60833-185, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-village-lumma-4-quartos-1-vaga-na-garagem-5-wc-wc-emp-sala-cozinha-imovel-caixa-economica-federal-cef-1600171-1444404293134-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>346615</v>
+      </c>
+      <c r="B13" t="n">
+        <v>225</v>
+      </c>
+      <c r="C13" t="n">
+        <v>140</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>346615</v>
+      </c>
+      <c r="G13" t="n">
+        <v>322901.2</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>14/02/2024</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>10/04/2024</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>16751</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>RUA CAPITAO VASCONCELOS N 1067,N. 1067 LT 02 QD 01, AEROLANDIA - CEP: 60850-680, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-lot-pq-santos-dumont-3-quartos-2-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1600170-1444405703298-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>283000</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="n">
+        <v>283000</v>
+      </c>
+      <c r="G14" t="n">
+        <v>169800</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>14/02/2024</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>10/04/2024</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>104576</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>RUA CORONEL JOAO DE OLIVEIRA N 555 APTO 318 B,N. 555 APTO. 318 TORRE B, MESSEJANA - CEP: 60841-820, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-res-villa-firenze-2-quartos-1-vaga-na-garagem-2-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1600167-1787700250099-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>330954.16</v>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>64.45</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>330954.16</v>
+      </c>
+      <c r="G15" t="n">
+        <v>317591.84</v>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>14/02/2024</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>02/04/2024</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>11/04/2024</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>13823</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>AVENIDA PRUDENTE BRASIL N 1200 010,N. 1200 0, PASSARE - CEP: 60743-770, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-residencial-passare-2-quartos-2-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1600163-1444416850181-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>222870</v>
+      </c>
+      <c r="B16" t="n">
+        <v>198</v>
+      </c>
+      <c r="C16" t="n">
+        <v>110</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="n">
+        <v>345000</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>25/09/2023</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>77065</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>7295618</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>RUA MARIA PINHEIRO CAMPELO,N. 720, LAGOA REDONDA - CEP: 60831-480, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-lagoa-redonda-1-vaga-na-garagem-equipamento-de-seguranca-imovel-caixa-economica-federal-cef-1462205-1444408426546-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>452200</v>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="n">
+        <v>195.47</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="n">
+        <v>700000</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>26/06/2023</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>33673</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>3500241</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>RUA GENERAL TERTULIANO POTIGUARA,N. 340 APTO. 302, ALDEOTA - CEP: 60135-280, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-ed-neptuno-3-quartos-2-vagas-na-garagem-area-de-servico-3-wc-wc-emp-sal-imovel-caixa-economica-federal-cef-1356406-1444406588166-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>147000</v>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="n">
+        <v>69.64</v>
+      </c>
+      <c r="D18" t="n">
+        <v>4</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="n">
+        <v>147000</v>
+      </c>
+      <c r="G18" t="n">
+        <v>119482.71</v>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>26/02/2024</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>23/04/2024</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>02/05/2024</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>58165</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>4852796</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>RUA FRANCISCO NOGUEIRA NUMERO 340 APARTAMENTO 202,N. 340 APTO. 202 BLOCO 12, CAJAZEIRAS - CEP: 60864-330, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-morada-das-acacias-a-4-quartos-1-vaga-na-garagem-3-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1613970-1444402277484-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>177000</v>
+      </c>
+      <c r="B19" t="n">
+        <v>200</v>
+      </c>
+      <c r="C19" t="n">
+        <v>135</v>
+      </c>
+      <c r="D19" t="n">
+        <v>5</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" t="n">
+        <v>177000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>129502.55</v>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>26/02/2024</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>29/04/2024</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>08/05/2024</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>13343</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>621137</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>RUA 11 N 40,N. 40 0, PREFEITO JOSE WALTER - CEP: 60750-250, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-conj-hab-prefeito-jose-walter-cavalcante-5-quartos-3-vagas-na-garagem-5-wc-imovel-caixa-economica-federal-cef-1613968-1555514958418-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>176180</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>176180</v>
+      </c>
+      <c r="G20" t="n">
+        <v>211907.1</v>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>26/02/2024</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>29/04/2024</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>08/05/2024</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>33715</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>6390528</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>RUA DOUTOR PEDRO SAMPAIO N 250 202 IITIPO B,N. 250 APTO. 202 BLOCO 2, PASSARE - CEP: 60861-500, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-condominium-seculus-imovel-caixa-economica-federal-cef-1613964-8444400967198-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>175000</v>
+      </c>
+      <c r="B21" t="n">
+        <v>100</v>
+      </c>
+      <c r="C21" t="n">
+        <v>85.02</v>
+      </c>
+      <c r="D21" t="n">
+        <v>2</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="n">
+        <v>175000</v>
+      </c>
+      <c r="G21" t="n">
+        <v>198554.19</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>09/04/2024</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>18/04/2024</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>36505</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>RUA JOAO MELO,N. 171 LT8 QD 32, BARROSO - CEP: 60862-725, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-barroso-2-quartos-2-vagas-na-garagem-2-wc-wc-emp-sala-cozinha-imovel-caixa-economica-federal-cef-1605340-8555515338993-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>863830</v>
+      </c>
+      <c r="B22" t="n">
+        <v>620.16</v>
+      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>863830</v>
+      </c>
+      <c r="G22" t="n">
+        <v>529046.74</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>15/04/2024</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>24/04/2024</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>32001</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>RUA ANA NERI,N. 316 LT 17 QD 06, JARDIM AMERICA - CEP: 60416-020, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/terreno-terreno-imovel-caixa-economica-federal-cef-1605337-1555514560597-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>172517.1</v>
+      </c>
+      <c r="B23" t="n">
+        <v>217.8</v>
+      </c>
+      <c r="C23" t="n">
+        <v>85.43000000000001</v>
+      </c>
+      <c r="D23" t="n">
+        <v>4</v>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>172517.1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>189525.13</v>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>15/04/2024</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>24/04/2024</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>53243</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>RUA MORADA NOVA,N. 414 LT12B QD 43, JANGURUSSU - CEP: 60870-610, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-jangurussu-4-quartos-4-wc-lavabo-imovel-caixa-economica-federal-cef-1605335-8444411848063-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>162880</v>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="n">
+        <v>41.54</v>
+      </c>
+      <c r="D24" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" t="n">
+        <v>162880</v>
+      </c>
+      <c r="G24" t="n">
+        <v>91403.84</v>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>15/04/2024</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>24/04/2024</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>83873</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>ESTRADA VELHA DO MURARA,N. 101 APTO. 101 BL 11 TP B TERREO, MESSEJANA - CEP: 60872-690, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-ideal-vila-dos-sonhos-2-quartos-1-vaga-na-garagem-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1605333-8555524832920-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>156000</v>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="n">
+        <v>44.11</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>156000</v>
+      </c>
+      <c r="G25" t="n">
+        <v>161168.54</v>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>15/04/2024</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>24/04/2024</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>65166</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>8900523</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>RUA MONTE LIBANO,N. 946 APTO. 301 BL 05, MONDUBIM - CEP: 60762-376, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-res-parque-fluence-1-vaga-na-garagem-imovel-caixa-economica-federal-cef-1605331-8787701148970-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>154400</v>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="n">
+        <v>54.75</v>
+      </c>
+      <c r="D26" t="n">
+        <v>3</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>154400</v>
+      </c>
+      <c r="G26" t="n">
+        <v>159553.1</v>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>15/04/2024</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>24/04/2024</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>35910</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>RUA MOREIRA DA ROCHA,N. 521 APTO. 103 1PAV, MONDUBIM - CEP: 60762-370, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-edificio-status-3-quartos-3-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1605330-8444415933910-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>115142</v>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="n">
+        <v>43.03</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1</v>
+      </c>
+      <c r="F27" t="n">
+        <v>115142</v>
+      </c>
+      <c r="G27" t="n">
+        <v>151345.61</v>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>19/02/2024</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>09/04/2024</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>18/04/2024</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>43565</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>7931409</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>RUA HERCULANO PENA,N. 101 APTO. 101 BL E, PARQUE PRESIDENTE VARGAS - CEP: 60765-525, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-res-manna-2-quartos-1-vaga-na-garagem-2-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1605329-8444411850394-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>200000</v>
+      </c>
+      <c r="B28" t="n">
+        <v>217.14</v>
+      </c>
+      <c r="C28" t="n">
+        <v>85.94</v>
+      </c>
+      <c r="D28" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="n">
+        <v>200000</v>
+      </c>
+      <c r="G28" t="n">
+        <v>124412.49</v>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>14/02/2024</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>10/04/2024</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>50137</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>2993490</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>RUA NOVA N 252,N. 252 LT 15 QD 22, JANGURUSSU - CEP: 60865-065, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-pq-santa-filomena-3-quartos-3-wc-sala-imovel-caixa-economica-federal-cef-1600168-8444408677814-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>173078</v>
+      </c>
+      <c r="B29" t="n">
+        <v>200</v>
+      </c>
+      <c r="C29" t="n">
+        <v>69.09</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
+        <v>173078</v>
+      </c>
+      <c r="G29" t="n">
+        <v>326202.87</v>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>14/02/2024</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>10/04/2024</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>84136</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>RUA I N 940,N. 940 LT 02 QD 20, MESSEJANA - CEP: 60000-000, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-lot-cidade-verde-2-quartos-2-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1600166-1444404237668-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>188000</v>
+      </c>
+      <c r="B30" t="n">
+        <v>264</v>
+      </c>
+      <c r="C30" t="n">
+        <v>64.81</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="n">
+        <v>188000</v>
+      </c>
+      <c r="G30" t="n">
+        <v>446034.11</v>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>14/02/2024</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>02/04/2024</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>11/04/2024</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>47487</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>RUA GIOVANNI BATISTA MONTINI N 647 647,N. 647 0, PARQUE DOIS IRMAOS - CEP: 60861-380, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-lt-c-2-quartos-2-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1600165-1444407119186-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>107596.25</v>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="n">
+        <v>43.03</v>
+      </c>
+      <c r="D31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F31" t="n">
+        <v>107596.25</v>
+      </c>
+      <c r="G31" t="n">
+        <v>85701.53999999999</v>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>14/02/2024</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>01/04/2024</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>10/04/2024</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>48655</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>8251851</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>RUA HERCULANO PENA N 101 APTO 103 BLOCO G,N. 101 APTO. 103 BL C, PARQUE PRESIDENTE VARGAS - CEP: 60765-525, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-res-manna-2-quartos-1-vaga-na-garagem-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1600164-8444406686581-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>196605.18</v>
+      </c>
+      <c r="B32" t="n">
+        <v>198</v>
+      </c>
+      <c r="C32" t="n">
+        <v>62.28</v>
+      </c>
+      <c r="D32" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="n">
+        <v>196605.18</v>
+      </c>
+      <c r="G32" t="n">
+        <v>279872.39</v>
+      </c>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>23/12/2023</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>03/06/2024</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>12/06/2024</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>5450</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>40931</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>RUA MARIO CAMPOS,N. 559 0, JARDIM GUANABARA - CEP: 60346-215, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-jardim-guanabara-2-quartos-varanda-sacada-wc-sala-cozinha-imovel-caixa-economica-federal-cef-1555098-1444406142893-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>93000</v>
+      </c>
+      <c r="B33" t="n">
+        <v>3960</v>
+      </c>
+      <c r="C33" t="n">
+        <v>44</v>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="n">
+        <v>155000</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>19/12/2023</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Leilão Caixa </t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>94356</t>
+        </is>
+      </c>
+      <c r="O33" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>RUA RUA DONA MENDINHA, N. 1025, APARTAMENTO 214, B,N. 1025 APTO. 214 BL A, CRISTO REDENTOR - CEP: 60337-385, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-residencial-francisco-de-as-1-vaga-na-garagem-imovel-caixa-economica-federal-cef-1549734-8444418473723-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>76479.60000000001</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="n">
+        <v>46.42</v>
+      </c>
+      <c r="D34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="n">
+        <v>138000</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>15/12/2023</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>05/03/2024</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>37732</t>
+        </is>
+      </c>
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>RUA 3,N. 350 APTO. 1 TIPO A, TORRE 02, PEDRAS - CEP: 60878-045, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-jardim-das-margaridas-2-quartos-1-vaga-na-garagem-varanda-sacada-are-imovel-caixa-economica-federal-cef-1547283-8555517180190-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>93116.39999999999</v>
+      </c>
+      <c r="B35" t="n">
+        <v>132</v>
+      </c>
+      <c r="C35" t="n">
+        <v>72.98999999999999</v>
+      </c>
+      <c r="D35" t="n">
+        <v>2</v>
+      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="n">
+        <v>156000</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>24/08/2023</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>96965</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>8994285</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>RUA ORLANDO DIAS,N. 230 BAIRRO GRANJA LISBOA, SIQUEIRA - CEP: 60544-420, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-siqueira-2-quartos-area-de-servico-wc-sala-cozinha-casa-geminada-imovel-caixa-economica-federal-cef-1422628-8444424595088-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>99172.5</v>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="n">
+        <v>63.1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="n">
+        <v>175000</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>19/08/2023</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>035709</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>6390498</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>RUA DOUTOR PEDRO SAMPAIO,N. 250 APTO. 102 BL II, PASSARE - CEP: 60861-500, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-cond-seculus-3-quartos-area-de-servico-2-wc-sala-equipamento-de-seguranc-imovel-caixa-economica-federal-cef-1416890-8555512757910-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>413440</v>
+      </c>
+      <c r="B37" t="n">
+        <v>277.22</v>
+      </c>
+      <c r="C37" t="n">
+        <v>221.4</v>
+      </c>
+      <c r="D37" t="n">
+        <v>3</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="n">
+        <v>640000</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>15/08/2023</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>83039</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>8006172</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>RUA TEOFREDO GOIANA,N. 295 QD 21, CIDADE DOS FUNCIONARIOS - CEP: 60822-630, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-lot-cidade-dos-funcionarios-3-quartos-3-vagas-na-garagem-3-varandas-sacada-imovel-caixa-economica-federal-cef-1412037-1444403855368-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>831402</v>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>174.82</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="n">
+        <v>1287000</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>18/07/2023</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>68471</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>3491463</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>A RUI BARBOSA,N. 1645 APTO. 302 AP302,, ALDEOTA - CEP: 60115-221, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-aldeota-3-quartos-1-vaga-na-garagem-3-wc-wc-emp-sala-dce-cozinha-pisc-imovel-caixa-economica-federal-cef-1380788-1555519457638-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>193800</v>
+      </c>
+      <c r="B39" t="n">
+        <v>117.35</v>
+      </c>
+      <c r="C39" t="n">
+        <v>115.15</v>
+      </c>
+      <c r="D39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3</v>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="n">
+        <v>360000</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>18/07/2023</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>89747</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>897471</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>RUA C,N. 582 UNIDADE A,, LAGOA REDONDA - CEP: 60831-227, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-lagoa-redonda-3-quartos-3-vagas-na-garagem-area-de-servico-3-wc-sala-co-imovel-caixa-economica-federal-cef-1380779-8444411287720-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>222224</v>
+      </c>
+      <c r="B40" t="n">
+        <v>136.13</v>
+      </c>
+      <c r="C40" t="n">
+        <v>266.26</v>
+      </c>
+      <c r="D40" t="n">
+        <v>5</v>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="n">
+        <v>344000</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>13/07/2023</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>23692</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>3571777</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>RUA MOACIR,N. 477, BARRA DO CEARA - CEP: 60332-650, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/residencial-barra-do-ceara-5-quartos-varanda-sacada-2-areas-de-servico-4-wc-4-salas-imovel-caixa-economica-federal-cef-1376345-1444400769657-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>518738</v>
+      </c>
+      <c r="B41" t="n">
+        <v>1617</v>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="n">
+        <v>803000</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>13/07/2023</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>01/03/2024</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Veras Negócios e Investimentos Ltda
+</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>52506</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>2218348</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>RUA ZACARIAS FLORINDO,N. S/N QD 104, LOTES 25, 26 E 27, GRANJA PORTUGAL - CEP: 60545-272, FORTALEZA - CEARA</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>https://www.leilaoimovel.com.br/imovel/ce/fortaleza/terreno-granja-portugal-imovel-caixa-economica-federal-cef-1376335-1444402490587-venda-direta-caixa</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>